<commit_message>
verify the result with optimized STvEA (using NearestNeighbors) and previous version. The result is consistent.
</commit_message>
<xml_diff>
--- a/Tests/test_scalability/1st Test/speed_scalability_test.xlsx
+++ b/Tests/test_scalability/1st Test/speed_scalability_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhangliangyang/Library/CloudStorage/OneDrive-Personal/研究相关/STvEA_Python/Tests/test_scalability/1st Test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6890C3-4213-9441-AF76-512E02FDF811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231A2467-4B5C-CF42-A19B-70AE8189857D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="22140" windowHeight="13480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12774,7 +12774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="133" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="133" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="U3" sqref="U3:Y5"/>
     </sheetView>
   </sheetViews>

</xml_diff>